<commit_message>
can ignore RUIDs now
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amulyamummaneni/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amulyamummaneni/Documents/emailList/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,22 +27,127 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>asm229</t>
+  </si>
+  <si>
+    <t>sao93</t>
+  </si>
+  <si>
+    <t>Dty15</t>
+  </si>
+  <si>
+    <t>jkl130@scarletmail.rutgers.edu</t>
+  </si>
+  <si>
+    <t>rr1031</t>
+  </si>
+  <si>
+    <t>js2335</t>
+  </si>
+  <si>
+    <t>jnm145</t>
+  </si>
+  <si>
+    <t>zaa23</t>
+  </si>
+  <si>
+    <t>nsk62</t>
+  </si>
+  <si>
+    <t>kem300</t>
+  </si>
+  <si>
+    <t>mr1411</t>
+  </si>
+  <si>
+    <t>sf595</t>
+  </si>
+  <si>
+    <t>jrb363</t>
+  </si>
+  <si>
+    <t>bpc64</t>
+  </si>
+  <si>
+    <t>acz14</t>
+  </si>
+  <si>
+    <t>stp76</t>
+  </si>
+  <si>
+    <t>aab289</t>
+  </si>
+  <si>
+    <t>jq89</t>
+  </si>
+  <si>
+    <t>jg1473</t>
+  </si>
+  <si>
+    <t>gft13</t>
+  </si>
+  <si>
+    <t>rra76</t>
+  </si>
+  <si>
+    <t>epr29</t>
+  </si>
+  <si>
+    <t>mcs319</t>
+  </si>
+  <si>
+    <t>nty4</t>
+  </si>
+  <si>
+    <t>sbm125</t>
+  </si>
+  <si>
+    <t>nrc64</t>
+  </si>
+  <si>
+    <t>el574</t>
+  </si>
+  <si>
+    <t>cvc47</t>
+  </si>
+  <si>
+    <t>mt958</t>
+  </si>
+  <si>
+    <t>xc259</t>
+  </si>
+  <si>
+    <t>mwz7</t>
+  </si>
+  <si>
+    <t>ajk260</t>
+  </si>
+  <si>
+    <t>sg1416</t>
+  </si>
+  <si>
+    <t>mjy37</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,8 +170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,27 +450,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1">
+        <v>185003648</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>189004305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>170004650</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>186003199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>190005115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>184008226</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>69003814</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>